<commit_message>
Refactor apartment model name, update payment upload instructions, enhance CSS styles, and improve payment API functionality
</commit_message>
<xml_diff>
--- a/files/payment-upload-from-xls.xlsx
+++ b/files/payment-upload-from-xls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yonapp-1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9652D981-48C3-4455-BCAF-31F62CA81FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3174BA-5740-4A61-B930-31651E094540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,6 +141,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7AD6E0"/>
+      <color rgb="FFAEE6EC"/>
+      <color rgb="FFEBEBED"/>
+      <color rgb="FFDFDEE2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -150,6 +158,328 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>847724</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Dikdörtgen: Köşeleri Yuvarlatılmış 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEAB17C7-6D1E-FC73-C300-8A60E10306E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10315574" y="485775"/>
+          <a:ext cx="5667375" cy="1638300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3955"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="AEE6EC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="7AD6E0"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="tr-TR" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4600575" cy="1642373"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Metin kutusu 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8906C8A-8E99-F2BB-0463-46767B84F45F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11258550" y="561975"/>
+          <a:ext cx="4600575" cy="1642373"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Açıklamalar:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="tr-TR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Daire kodu</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> -&gt; Daire kaydı yaparken oluşturulan daire kodu</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>** Açıklama alanı içinde daire kodu geçiyorsa daire kodu yazmanıza gerek yoktur,</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>**Bir satırda birden fazla tahsilat türü var ise o kaydı satırlara bölerek yükleyin</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>         (Örnek : Aidat ve Demirbaşı tek seferde gönderdi ama siz ayrı ayrı işlemek istiyorsanız o kaydı iki satır haline getirip yükleyin)</a:t>
+          </a:r>
+          <a:endParaRPr lang="tr-TR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="tr-TR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4" descr="Bilgi ana hat">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACF4591-FF9D-C571-F5B1-4C36C23AD8C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10467975" y="923925"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,7 +748,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +784,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add PHPUnit support and initial test setup
</commit_message>
<xml_diff>
--- a/files/payment-upload-from-xls.xlsx
+++ b/files/payment-upload-from-xls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yonapp-1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3174BA-5740-4A61-B930-31651E094540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F0D368-6FB7-4056-B8AC-B9BAC94E742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,12 +65,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{41373B60-7700-4B5C-B936-F18D89DFFA9C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>YONAPP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+*Ev Sahibi
+*Kiracı
+*Diğer</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Tarih</t>
   </si>
@@ -85,6 +111,12 @@
   </si>
   <si>
     <t>Daire Kodu</t>
+  </si>
+  <si>
+    <t>Ödeme Türü</t>
+  </si>
+  <si>
+    <t>Ödeyen</t>
   </si>
 </sst>
 </file>
@@ -164,16 +196,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>847724</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>866774</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -188,8 +220,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10315574" y="485775"/>
-          <a:ext cx="5667375" cy="1638300"/>
+          <a:off x="11858624" y="438149"/>
+          <a:ext cx="5667375" cy="2352676"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -238,12 +270,12 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4600575" cy="1642373"/>
+    <xdr:ext cx="4600575" cy="2171700"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="Metin kutusu 2">
@@ -257,8 +289,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11258550" y="561975"/>
-          <a:ext cx="4600575" cy="1642373"/>
+          <a:off x="12287250" y="561975"/>
+          <a:ext cx="4600575" cy="2171700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -281,7 +313,7 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
@@ -418,6 +450,68 @@
             </a:rPr>
             <a:t>         (Örnek : Aidat ve Demirbaşı tek seferde gönderdi ama siz ayrı ayrı işlemek istiyorsanız o kaydı iki satır haline getirip yükleyin)</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>**Ödeyen-&gt; Varsayılan olarak Ev Sahibi kaydedilir.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>** Ödeme Türü-&gt; Aidat, Demirbaş gibi daha önce tanımladığınız borçlandırma türlerinden birini yazınız</a:t>
+          </a:r>
           <a:endParaRPr lang="tr-TR">
             <a:effectLst/>
           </a:endParaRPr>
@@ -431,16 +525,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -469,7 +563,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10467975" y="923925"/>
+          <a:off x="11506200" y="1133475"/>
           <a:ext cx="762000" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -745,26 +839,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -775,9 +869,15 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor(session): centralize session configuration and initialization
feat(duyuru): add edit functionality for announcements
feat(anket): improve survey management with edit and status features
feat(payment): enhance payment processing with income/expense categories
fix(validation): fix select2 validation for specific elements
style(css): adjust cursor styling for move arrows
docs: update various documentation and comments
</commit_message>
<xml_diff>
--- a/files/payment-upload-from-xls.xlsx
+++ b/files/payment-upload-from-xls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yonapp-1\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F0D368-6FB7-4056-B8AC-B9BAC94E742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F970A248-BC24-4268-AF05-5B3EE962947F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,390 +190,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>866774</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Dikdörtgen: Köşeleri Yuvarlatılmış 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEAB17C7-6D1E-FC73-C300-8A60E10306E0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11858624" y="438149"/>
-          <a:ext cx="5667375" cy="2352676"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 3955"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="AEE6EC"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="7AD6E0"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="tr-TR" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4600575" cy="2171700"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Metin kutusu 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8906C8A-8E99-F2BB-0463-46767B84F45F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12287250" y="561975"/>
-          <a:ext cx="4600575" cy="2171700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Açıklamalar:</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="tr-TR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Daire kodu</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> -&gt; Daire kaydı yaparken oluşturulan daire kodu</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>** Açıklama alanı içinde daire kodu geçiyorsa daire kodu yazmanıza gerek yoktur,</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>**Bir satırda birden fazla tahsilat türü var ise o kaydı satırlara bölerek yükleyin</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>         (Örnek : Aidat ve Demirbaşı tek seferde gönderdi ama siz ayrı ayrı işlemek istiyorsanız o kaydı iki satır haline getirip yükleyin)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>**Ödeyen-&gt; Varsayılan olarak Ev Sahibi kaydedilir.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>** Ödeme Türü-&gt; Aidat, Demirbaş gibi daha önce tanımladığınız borçlandırma türlerinden birini yazınız</a:t>
-          </a:r>
-          <a:endParaRPr lang="tr-TR">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="tr-TR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Grafik 4" descr="Bilgi ana hat">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ACF4591-FF9D-C571-F5B1-4C36C23AD8C3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11506200" y="1133475"/>
-          <a:ext cx="762000" cy="762000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -842,7 +458,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +500,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>